<commit_message>
AutoCommit_10 октября 2023 г. 9:13:09_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>2ОИБАС1222: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Инд1</t>
+  </si>
+  <si>
+    <t>Лаб1</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -536,7 +539,9 @@
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -560,7 +565,9 @@
         <v>1</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -575,7 +582,9 @@
         <v>2</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -605,7 +614,9 @@
         <v>4</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -635,7 +646,9 @@
         <v>6</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -680,7 +693,9 @@
         <v>9</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -740,7 +755,9 @@
         <v>13</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -832,7 +849,9 @@
       <c r="C23" s="2">
         <v>5</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -847,7 +866,9 @@
         <v>20</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -877,7 +898,9 @@
         <v>22</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2">
+        <v>5</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -892,7 +915,9 @@
         <v>23</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>5</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -907,7 +932,9 @@
         <v>24</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -937,7 +964,9 @@
         <v>26</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_23 октября 2023 г. 10:19:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -503,10 +503,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -677,7 +677,9 @@
         <v>5</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -966,7 +968,9 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -983,7 +987,9 @@
       <c r="D30" s="2">
         <v>5</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_23 октября 2023 г. 10:27:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -503,10 +503,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -659,7 +659,9 @@
       <c r="D10" s="2">
         <v>5</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -693,7 +695,9 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -742,7 +746,9 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -774,7 +780,9 @@
       <c r="D17" s="2">
         <v>5</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -870,7 +878,9 @@
       <c r="D23" s="2">
         <v>5</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -902,7 +912,9 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -919,7 +931,9 @@
       <c r="D26" s="2">
         <v>5</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -936,7 +950,9 @@
       <c r="D27" s="2">
         <v>5</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -953,7 +969,9 @@
       <c r="D28" s="2">
         <v>5</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2">
+        <v>5</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_23 октября 2023 г. 10:33:35_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -503,10 +503,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -578,7 +578,9 @@
       <c r="D5" s="2">
         <v>5</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -627,7 +629,9 @@
       <c r="D8" s="2">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -642,7 +646,9 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -674,7 +680,9 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
       <c r="D11" s="2">
         <v>5</v>
       </c>
@@ -910,7 +918,9 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2">
         <v>5</v>
@@ -1035,7 +1045,9 @@
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2">
+        <v>5</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 15:13:03_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -503,10 +503,10 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -769,7 +769,9 @@
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -865,7 +867,9 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -994,7 +998,9 @@
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2">
+        <v>5</v>
+      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 15:45:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -506,7 +506,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -597,8 +597,12 @@
       <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -612,8 +616,12 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -855,7 +863,9 @@
       <c r="E21" s="2">
         <v>5</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -948,7 +958,9 @@
       <c r="E26" s="2">
         <v>5</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="2">
+        <v>5</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -967,7 +979,9 @@
       <c r="E27" s="2">
         <v>5</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1001,7 +1015,9 @@
       <c r="C29" s="2">
         <v>5</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
       <c r="E29" s="2">
         <v>5</v>
       </c>
@@ -1054,9 +1070,15 @@
       <c r="C32" s="2">
         <v>5</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>5</v>
+      </c>
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 16:01:52_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>2ОИБАС1222: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>Инд3</t>
+  </si>
+  <si>
+    <t>Шаповаленко</t>
+  </si>
+  <si>
+    <t>Лаб2</t>
+  </si>
+  <si>
+    <t>Лаб3-4</t>
+  </si>
+  <si>
+    <t>Лаб5</t>
   </si>
 </sst>
 </file>
@@ -183,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -193,6 +205,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -500,13 +518,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -517,57 +535,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-    </row>
-    <row r="3" spans="1:23" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+    </row>
+    <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -578,15 +601,14 @@
       <c r="D5" s="2">
         <v>5</v>
       </c>
-      <c r="E5" s="2">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -603,11 +625,10 @@
       <c r="F6" s="2">
         <v>5</v>
       </c>
-      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -615,18 +636,19 @@
         <v>3</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
       <c r="E7" s="2">
         <v>5</v>
       </c>
       <c r="F7" s="2">
         <v>5</v>
       </c>
-      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -637,15 +659,14 @@
       <c r="D8" s="2">
         <v>5</v>
       </c>
-      <c r="E8" s="2">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -653,16 +674,17 @@
         <v>5</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -673,15 +695,14 @@
       <c r="D10" s="2">
         <v>5</v>
       </c>
-      <c r="E10" s="2">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -691,18 +712,17 @@
       <c r="C11" s="2">
         <v>5</v>
       </c>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
       <c r="F11" s="2">
         <v>5</v>
       </c>
-      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -710,16 +730,15 @@
         <v>8</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -727,16 +746,15 @@
         <v>9</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -745,15 +763,14 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2"/>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -761,16 +778,15 @@
         <v>11</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:23" ht="13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -782,12 +798,13 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -798,15 +815,14 @@
       <c r="D17" s="2">
         <v>5</v>
       </c>
-      <c r="E17" s="2">
-        <v>5</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
+        <v>5</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -816,12 +832,13 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -832,11 +849,10 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -847,11 +863,10 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -859,18 +874,19 @@
         <v>17</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2">
+        <v>5</v>
+      </c>
       <c r="E21" s="2">
         <v>5</v>
       </c>
       <c r="F21" s="2">
         <v>5</v>
       </c>
-      <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -882,12 +898,13 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -900,15 +917,14 @@
       <c r="D23" s="2">
         <v>5</v>
       </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -916,16 +932,15 @@
         <v>20</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="F24" s="2">
+        <v>5</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -935,16 +950,15 @@
       <c r="C25" s="2">
         <v>5</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2">
-        <v>5</v>
-      </c>
+      <c r="D25" s="2">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -961,11 +975,10 @@
       <c r="F26" s="2">
         <v>5</v>
       </c>
-      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -982,11 +995,10 @@
       <c r="F27" s="2">
         <v>5</v>
       </c>
-      <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -997,15 +1009,14 @@
       <c r="D28" s="2">
         <v>5</v>
       </c>
-      <c r="E28" s="2">
-        <v>5</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2">
+        <v>5</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1018,15 +1029,14 @@
       <c r="D29" s="2">
         <v>5</v>
       </c>
-      <c r="E29" s="2">
-        <v>5</v>
-      </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1037,15 +1047,14 @@
       <c r="D30" s="2">
         <v>5</v>
       </c>
-      <c r="E30" s="2">
-        <v>5</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1055,12 +1064,13 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="F31" s="2">
+        <v>5</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -1079,18 +1089,24 @@
       <c r="F32" s="2">
         <v>5</v>
       </c>
-      <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="2:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="5">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_6 ноября 2023 г. 16:03:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>2ОИБАС1222: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Лаб5</t>
+  </si>
+  <si>
+    <t>Лаб6</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -582,6 +585,9 @@
       <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
@@ -699,8 +705,14 @@
       <c r="F10" s="2">
         <v>5</v>
       </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
+      <c r="J10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -720,7 +732,9 @@
         <v>5</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="I11" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -768,7 +782,9 @@
       </c>
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -884,7 +900,9 @@
         <v>5</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -976,7 +994,9 @@
         <v>5</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="I26" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -996,7 +1016,9 @@
         <v>5</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="I27" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -1014,7 +1036,9 @@
         <v>5</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="I28" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -1067,7 +1091,9 @@
       <c r="F31" s="2">
         <v>5</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="2">
+        <v>5</v>
+      </c>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_8 ноября 2023 г. 9:09:57_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -224,9 +224,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -534,10 +534,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="I28" activeCellId="3" sqref="I21 I26 I27 I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -548,29 +548,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -715,7 +715,7 @@
       <c r="F10" s="6">
         <v>5</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>5</v>
       </c>
       <c r="H10" s="2"/>
@@ -742,7 +742,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="2">
+      <c r="I11" s="6">
         <v>5</v>
       </c>
     </row>
@@ -792,7 +792,7 @@
       </c>
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2">
+      <c r="I14" s="6">
         <v>5</v>
       </c>
     </row>
@@ -910,7 +910,7 @@
         <v>5</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="2">
+      <c r="I21" s="6">
         <v>5</v>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
         <v>5</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="2">
+      <c r="I26" s="6">
         <v>5</v>
       </c>
     </row>
@@ -1026,7 +1026,7 @@
         <v>5</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="2">
+      <c r="I27" s="6">
         <v>5</v>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
         <v>5</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="2">
+      <c r="I28" s="6">
         <v>5</v>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       <c r="F31" s="6">
         <v>5</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="6">
         <v>5</v>
       </c>
       <c r="I31" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 16:34:19_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -534,10 +534,10 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I28" activeCellId="3" sqref="I21 I26 I27 I28"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -707,7 +707,9 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
       <c r="D10" s="6">
         <v>5</v>
       </c>
@@ -734,7 +736,9 @@
       <c r="C11" s="6">
         <v>5</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
       <c r="E11" s="6">
         <v>5</v>
       </c>
@@ -757,7 +761,9 @@
       <c r="D12" s="6">
         <v>5</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -786,7 +792,9 @@
         <v>10</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
       <c r="E14" s="6">
         <v>5</v>
       </c>
@@ -803,11 +811,15 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
       <c r="D15" s="6">
         <v>5</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -822,8 +834,12 @@
       <c r="C16" s="6">
         <v>5</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
       <c r="F16" s="6">
         <v>5</v>
       </c>
@@ -857,7 +873,9 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
       <c r="F18" s="6">
         <v>5</v>
       </c>
@@ -899,7 +917,9 @@
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
       <c r="D21" s="6">
         <v>5</v>
       </c>
@@ -924,8 +944,12 @@
       <c r="C22" s="6">
         <v>5</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
       <c r="F22" s="6">
         <v>5</v>
       </c>
@@ -960,7 +984,9 @@
         <v>20</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="6">
         <v>5</v>
@@ -1037,7 +1063,9 @@
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2">
+        <v>5</v>
+      </c>
       <c r="D28" s="6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 16:44:54_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>2ОИБАС1222: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Лаб6</t>
+  </si>
+  <si>
+    <t>Инд4</t>
+  </si>
+  <si>
+    <t>еремин</t>
   </si>
 </sst>
 </file>
@@ -531,13 +537,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -584,27 +590,30 @@
         <v>32</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -618,11 +627,14 @@
         <v>5</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="6">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2"/>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5</v>
+      </c>
       <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -638,11 +650,11 @@
       <c r="E6" s="6">
         <v>5</v>
       </c>
-      <c r="F6" s="6">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2"/>
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
       <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -658,11 +670,11 @@
       <c r="E7" s="6">
         <v>5</v>
       </c>
-      <c r="F7" s="6">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2"/>
+      <c r="G7" s="6">
+        <v>5</v>
+      </c>
       <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -676,11 +688,11 @@
         <v>5</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="6">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2"/>
+      <c r="G8" s="6">
+        <v>5</v>
+      </c>
       <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -694,11 +706,14 @@
         <v>5</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="6">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2"/>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5</v>
+      </c>
       <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -714,15 +729,15 @@
         <v>5</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="6">
-        <v>5</v>
-      </c>
-      <c r="G10" s="7">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2"/>
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+      <c r="H10" s="7">
+        <v>5</v>
+      </c>
       <c r="I10" s="2"/>
-      <c r="J10">
+      <c r="J10" s="2"/>
+      <c r="K10">
         <v>5</v>
       </c>
     </row>
@@ -742,11 +757,11 @@
       <c r="E11" s="6">
         <v>5</v>
       </c>
-      <c r="F11" s="6">
-        <v>5</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="6">
+      <c r="G11" s="6">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="6">
         <v>5</v>
       </c>
     </row>
@@ -764,9 +779,9 @@
       <c r="E12" s="2">
         <v>5</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -778,11 +793,11 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="6">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2"/>
+      <c r="G13" s="6">
+        <v>5</v>
+      </c>
       <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -798,9 +813,9 @@
       <c r="E14" s="6">
         <v>5</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="6">
+      <c r="G14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="6">
         <v>5</v>
       </c>
     </row>
@@ -820,9 +835,9 @@
       <c r="E15" s="2">
         <v>5</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -840,13 +855,13 @@
       <c r="E16" s="2">
         <v>5</v>
       </c>
-      <c r="F16" s="6">
-        <v>5</v>
-      </c>
-      <c r="H16" s="2"/>
+      <c r="G16" s="6">
+        <v>5</v>
+      </c>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -858,13 +873,13 @@
         <v>5</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="6">
-        <v>5</v>
-      </c>
-      <c r="H17" s="2"/>
+      <c r="G17" s="6">
+        <v>5</v>
+      </c>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -876,13 +891,13 @@
       <c r="E18" s="2">
         <v>5</v>
       </c>
-      <c r="F18" s="6">
-        <v>5</v>
-      </c>
-      <c r="H18" s="2"/>
+      <c r="G18" s="6">
+        <v>5</v>
+      </c>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -892,11 +907,11 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="G19" s="2"/>
       <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -906,11 +921,11 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="G20" s="2"/>
       <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -926,15 +941,15 @@
       <c r="E21" s="6">
         <v>5</v>
       </c>
-      <c r="F21" s="6">
-        <v>5</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="6">
+        <v>5</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -950,13 +965,13 @@
       <c r="E22" s="2">
         <v>5</v>
       </c>
-      <c r="F22" s="6">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2"/>
+      <c r="G22" s="6">
+        <v>5</v>
+      </c>
       <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -969,14 +984,16 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="6">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2"/>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
+      <c r="G23" s="6">
+        <v>5</v>
+      </c>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -987,14 +1004,16 @@
       <c r="D24" s="2">
         <v>5</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="6">
-        <v>5</v>
-      </c>
-      <c r="H24" s="2"/>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="G24" s="6">
+        <v>5</v>
+      </c>
       <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1008,11 +1027,11 @@
         <v>5</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="G25" s="2"/>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -1026,15 +1045,15 @@
       <c r="E26" s="6">
         <v>5</v>
       </c>
-      <c r="F26" s="6">
-        <v>5</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="6">
+        <v>5</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1048,15 +1067,15 @@
       <c r="E27" s="6">
         <v>5</v>
       </c>
-      <c r="F27" s="6">
-        <v>5</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="6">
+        <v>5</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1070,15 +1089,15 @@
         <v>5</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="6">
-        <v>5</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="6">
+        <v>5</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1091,14 +1110,16 @@
       <c r="D29" s="6">
         <v>5</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="6">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2"/>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
+      <c r="G29" s="6">
+        <v>5</v>
+      </c>
       <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1109,14 +1130,16 @@
       <c r="D30" s="6">
         <v>5</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="6">
-        <v>5</v>
-      </c>
-      <c r="H30" s="2"/>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="G30" s="6">
+        <v>5</v>
+      </c>
       <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1126,15 +1149,15 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="6">
-        <v>5</v>
-      </c>
-      <c r="H31" s="6">
-        <v>5</v>
-      </c>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="6">
+        <v>5</v>
+      </c>
+      <c r="I31" s="6">
+        <v>5</v>
+      </c>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -1150,25 +1173,33 @@
       <c r="E32" s="6">
         <v>5</v>
       </c>
-      <c r="F32" s="6">
-        <v>5</v>
-      </c>
-      <c r="H32" s="2"/>
+      <c r="G32" s="6">
+        <v>5</v>
+      </c>
       <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="2:9" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="2:10" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="G33" s="3"/>
       <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="2:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="2:10" ht="13" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="5">
+      <c r="G34" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 17:03:51_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>2ОИБАС1222: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>еремин</t>
+  </si>
+  <si>
+    <t>никоноров</t>
+  </si>
+  <si>
+    <t>Инд5</t>
   </si>
 </sst>
 </file>
@@ -169,7 +175,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,8 +188,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -206,11 +218,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -231,6 +254,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -537,13 +566,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -554,29 +583,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -593,27 +622,30 @@
         <v>38</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -630,11 +662,11 @@
       <c r="F5">
         <v>5</v>
       </c>
-      <c r="G5" s="6">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2"/>
+      <c r="H5" s="6">
+        <v>5</v>
+      </c>
       <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -650,11 +682,11 @@
       <c r="E6" s="6">
         <v>5</v>
       </c>
-      <c r="G6" s="6">
-        <v>5</v>
-      </c>
-      <c r="I6" s="2"/>
+      <c r="H6" s="6">
+        <v>5</v>
+      </c>
       <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -670,11 +702,11 @@
       <c r="E7" s="6">
         <v>5</v>
       </c>
-      <c r="G7" s="6">
-        <v>5</v>
-      </c>
-      <c r="I7" s="2"/>
+      <c r="H7" s="6">
+        <v>5</v>
+      </c>
       <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -688,11 +720,11 @@
         <v>5</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="G8" s="6">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2"/>
+      <c r="H8" s="6">
+        <v>5</v>
+      </c>
       <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -709,11 +741,11 @@
       <c r="F9">
         <v>5</v>
       </c>
-      <c r="G9" s="6">
-        <v>5</v>
-      </c>
-      <c r="I9" s="2"/>
+      <c r="H9" s="6">
+        <v>5</v>
+      </c>
       <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -729,15 +761,15 @@
         <v>5</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="G10" s="6">
-        <v>5</v>
-      </c>
-      <c r="H10" s="7">
-        <v>5</v>
-      </c>
-      <c r="I10" s="2"/>
+      <c r="H10" s="6">
+        <v>5</v>
+      </c>
+      <c r="I10" s="7">
+        <v>5</v>
+      </c>
       <c r="J10" s="2"/>
-      <c r="K10">
+      <c r="K10" s="2"/>
+      <c r="L10">
         <v>5</v>
       </c>
     </row>
@@ -757,11 +789,11 @@
       <c r="E11" s="6">
         <v>5</v>
       </c>
-      <c r="G11" s="6">
-        <v>5</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="6">
+      <c r="H11" s="6">
+        <v>5</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="6">
         <v>5</v>
       </c>
     </row>
@@ -779,9 +811,11 @@
       <c r="E12" s="2">
         <v>5</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
       <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -793,11 +827,14 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="G13" s="6">
-        <v>5</v>
-      </c>
-      <c r="I13" s="2"/>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="H13" s="6">
+        <v>5</v>
+      </c>
       <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -813,9 +850,9 @@
       <c r="E14" s="6">
         <v>5</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="6">
+      <c r="H14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="6">
         <v>5</v>
       </c>
     </row>
@@ -835,9 +872,12 @@
       <c r="E15" s="2">
         <v>5</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15">
+        <v>5</v>
+      </c>
       <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -855,13 +895,13 @@
       <c r="E16" s="2">
         <v>5</v>
       </c>
-      <c r="G16" s="6">
-        <v>5</v>
-      </c>
-      <c r="I16" s="2"/>
+      <c r="H16" s="6">
+        <v>5</v>
+      </c>
       <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -873,13 +913,13 @@
         <v>5</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="G17" s="6">
-        <v>5</v>
-      </c>
-      <c r="I17" s="2"/>
+      <c r="H17" s="6">
+        <v>5</v>
+      </c>
       <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -891,13 +931,16 @@
       <c r="E18" s="2">
         <v>5</v>
       </c>
-      <c r="G18" s="6">
-        <v>5</v>
-      </c>
-      <c r="I18" s="2"/>
+      <c r="H18" s="6">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
       <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -907,11 +950,11 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="H19" s="2"/>
       <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -921,11 +964,11 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="H20" s="2"/>
       <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -941,15 +984,18 @@
       <c r="E21" s="6">
         <v>5</v>
       </c>
-      <c r="G21" s="6">
-        <v>5</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="6">
+        <v>5</v>
+      </c>
+      <c r="I21" s="9">
+        <v>5</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -965,13 +1011,13 @@
       <c r="E22" s="2">
         <v>5</v>
       </c>
-      <c r="G22" s="6">
-        <v>5</v>
-      </c>
-      <c r="I22" s="2"/>
+      <c r="H22" s="6">
+        <v>5</v>
+      </c>
       <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -987,13 +1033,13 @@
       <c r="E23" s="2">
         <v>5</v>
       </c>
-      <c r="G23" s="6">
-        <v>5</v>
-      </c>
-      <c r="I23" s="2"/>
+      <c r="H23" s="6">
+        <v>5</v>
+      </c>
       <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -1007,13 +1053,16 @@
       <c r="E24" s="2">
         <v>5</v>
       </c>
-      <c r="G24" s="6">
-        <v>5</v>
-      </c>
-      <c r="I24" s="2"/>
+      <c r="H24" s="6">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
       <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1027,11 +1076,19 @@
         <v>5</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="H25" s="2">
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
       <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -1045,15 +1102,15 @@
       <c r="E26" s="6">
         <v>5</v>
       </c>
-      <c r="G26" s="6">
-        <v>5</v>
-      </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="6">
+        <v>5</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1067,15 +1124,15 @@
       <c r="E27" s="6">
         <v>5</v>
       </c>
-      <c r="G27" s="6">
-        <v>5</v>
-      </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="6">
+        <v>5</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -1089,15 +1146,15 @@
         <v>5</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="G28" s="6">
-        <v>5</v>
-      </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="6">
+        <v>5</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -1113,13 +1170,19 @@
       <c r="E29" s="2">
         <v>5</v>
       </c>
-      <c r="G29" s="6">
-        <v>5</v>
-      </c>
-      <c r="I29" s="2"/>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29" s="6">
+        <v>5</v>
+      </c>
       <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -1133,13 +1196,13 @@
       <c r="E30" s="2">
         <v>5</v>
       </c>
-      <c r="G30" s="6">
-        <v>5</v>
-      </c>
-      <c r="I30" s="2"/>
+      <c r="H30" s="6">
+        <v>5</v>
+      </c>
       <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -1149,15 +1212,15 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="G31" s="6">
-        <v>5</v>
-      </c>
-      <c r="I31" s="6">
-        <v>5</v>
-      </c>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="6">
+        <v>5</v>
+      </c>
+      <c r="J31" s="6">
+        <v>5</v>
+      </c>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -1173,33 +1236,47 @@
       <c r="E32" s="6">
         <v>5</v>
       </c>
-      <c r="G32" s="6">
-        <v>5</v>
-      </c>
-      <c r="I32" s="2"/>
+      <c r="F32" s="8">
+        <v>5</v>
+      </c>
+      <c r="G32" s="8">
+        <v>5</v>
+      </c>
+      <c r="H32" s="6">
+        <v>5</v>
+      </c>
       <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="2:10" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="2:11" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="I33" s="3"/>
+      <c r="H33" s="3"/>
       <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="2:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="2:11" ht="13" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G34" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="H34" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="13" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 17:06:40_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -569,10 +569,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1085,9 @@
       <c r="I25">
         <v>5</v>
       </c>
-      <c r="J25" s="2"/>
+      <c r="J25" s="2">
+        <v>5</v>
+      </c>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1149,6 +1151,9 @@
       <c r="H28" s="6">
         <v>5</v>
       </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
       <c r="J28" s="2"/>
       <c r="K28" s="6">
         <v>5</v>
@@ -1177,6 +1182,9 @@
         <v>5</v>
       </c>
       <c r="H29" s="6">
+        <v>5</v>
+      </c>
+      <c r="I29">
         <v>5</v>
       </c>
       <c r="J29" s="2"/>
@@ -1243,6 +1251,9 @@
         <v>5</v>
       </c>
       <c r="H32" s="6">
+        <v>5</v>
+      </c>
+      <c r="I32" s="8">
         <v>5</v>
       </c>
       <c r="J32" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 17:14:09_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -569,10 +569,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -666,7 +666,9 @@
         <v>5</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -686,7 +688,9 @@
         <v>5</v>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="K6" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -706,7 +710,9 @@
         <v>5</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -724,7 +730,9 @@
         <v>5</v>
       </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -768,7 +776,9 @@
         <v>5</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2">
+        <v>5</v>
+      </c>
       <c r="L10">
         <v>5</v>
       </c>
@@ -834,7 +844,9 @@
         <v>5</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="K13" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -877,7 +889,9 @@
         <v>5</v>
       </c>
       <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="K15" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -917,7 +931,9 @@
         <v>5</v>
       </c>
       <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="K17" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -938,7 +954,9 @@
         <v>5</v>
       </c>
       <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="K18" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">

</xml_diff>

<commit_message>
AutoCommit_13 ноября 2023 г. 17:15:34_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -569,10 +569,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1055,9 @@
         <v>5</v>
       </c>
       <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="K23" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -1078,7 +1080,9 @@
         <v>5</v>
       </c>
       <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="K24" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -1106,7 +1110,9 @@
       <c r="J25" s="2">
         <v>5</v>
       </c>
-      <c r="K25" s="2"/>
+      <c r="K25" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -1206,7 +1212,9 @@
         <v>5</v>
       </c>
       <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="K29" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -1226,7 +1234,9 @@
         <v>5</v>
       </c>
       <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="K30" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
@@ -1275,7 +1285,9 @@
         <v>5</v>
       </c>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="K32" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="2:11" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_17 ноября 2023 г. 23:10:19_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -172,7 +172,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,12 +182,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -251,16 +245,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,10 +561,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -584,29 +575,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -693,7 +684,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5">
+      <c r="F5" s="7">
         <v>5</v>
       </c>
       <c r="H5" s="6">
@@ -711,11 +702,11 @@
         <f>IF($M5*2&gt;N$4,1,0)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="8">
         <f t="shared" ref="O5:P5" si="0">IF($M5*2&gt;O$4,1,0)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -744,19 +735,19 @@
       <c r="K6" s="2">
         <v>5</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="8">
         <f t="shared" ref="M6:M31" si="1">SUM(C6:K6)</f>
         <v>20</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="8">
         <f t="shared" ref="N6:P32" si="2">IF($M6*2&gt;N$4,1,0)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="10">
+      <c r="O6" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -785,19 +776,19 @@
       <c r="K7" s="2">
         <v>3</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="8">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="N7" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="10">
+      <c r="N7" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -824,19 +815,19 @@
       <c r="K8" s="2">
         <v>4</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="8">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="N8" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="10">
+      <c r="N8" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -856,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9">
+      <c r="F9" s="7">
         <v>5</v>
       </c>
       <c r="H9" s="6">
@@ -864,19 +855,19 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="M9" s="10">
+      <c r="M9" s="8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="N9" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="10">
+      <c r="N9" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -891,7 +882,7 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="6">
         <v>5</v>
       </c>
       <c r="D10" s="6">
@@ -908,19 +899,19 @@
       <c r="K10" s="2">
         <v>5</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="8">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="N10" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P10" s="10">
+      <c r="N10" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P10" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -938,7 +929,7 @@
       <c r="C11" s="6">
         <v>5</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="6">
         <v>5</v>
       </c>
       <c r="E11" s="6">
@@ -951,19 +942,19 @@
       <c r="K11" s="6">
         <v>5</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="8">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="N11" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P11" s="10">
+      <c r="N11" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P11" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -982,27 +973,27 @@
       <c r="D12" s="6">
         <v>5</v>
       </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="E12" s="6">
+        <v>5</v>
+      </c>
+      <c r="H12" s="6">
         <v>5</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="M12" s="10">
+      <c r="M12" s="8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="N12" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="10">
+      <c r="N12" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1020,7 +1011,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13">
+      <c r="F13" s="7">
         <v>5</v>
       </c>
       <c r="H13" s="6">
@@ -1030,19 +1021,19 @@
       <c r="K13" s="2">
         <v>5</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="N13" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="10">
+      <c r="N13" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1058,7 +1049,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2">
+      <c r="D14" s="6">
         <v>5</v>
       </c>
       <c r="E14" s="6">
@@ -1069,19 +1060,19 @@
       <c r="K14" s="6">
         <v>5</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="N14" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="10">
+      <c r="N14" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1096,36 +1087,36 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="6">
         <v>5</v>
       </c>
       <c r="D15" s="6">
         <v>5</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="6">
         <v>5</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15">
+      <c r="I15" s="7">
         <v>5</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2">
         <v>5</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="8">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="N15" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P15" s="10">
+      <c r="N15" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P15" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1143,10 +1134,10 @@
       <c r="C16" s="6">
         <v>5</v>
       </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="D16" s="6">
+        <v>5</v>
+      </c>
+      <c r="E16" s="6">
         <v>5</v>
       </c>
       <c r="H16" s="6">
@@ -1154,19 +1145,19 @@
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="M16" s="10">
+      <c r="M16" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="N16" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="10">
+      <c r="N16" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1193,19 +1184,19 @@
       <c r="K17" s="2">
         <v>4</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="8">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="N17" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="10">
+      <c r="N17" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1222,32 +1213,32 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2">
+      <c r="E18" s="6">
         <v>5</v>
       </c>
       <c r="H18" s="6">
         <v>5</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="7">
         <v>5</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2">
         <v>5</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="N18" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="10">
+      <c r="N18" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1268,19 +1259,19 @@
       <c r="H19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="M19" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="10">
+      <c r="M19" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1301,19 +1292,19 @@
       <c r="H20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="M20" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="10">
+      <c r="M20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1328,7 +1319,7 @@
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="6">
         <v>5</v>
       </c>
       <c r="D21" s="6">
@@ -1340,26 +1331,26 @@
       <c r="H21" s="6">
         <v>5</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="12">
         <v>5</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="6">
         <v>5</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="8">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="N21" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O21" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P21" s="10">
+      <c r="N21" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O21" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P21" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1377,10 +1368,10 @@
       <c r="C22" s="6">
         <v>5</v>
       </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="D22" s="6">
+        <v>5</v>
+      </c>
+      <c r="E22" s="6">
         <v>5</v>
       </c>
       <c r="H22" s="6">
@@ -1388,19 +1379,19 @@
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="M22" s="10">
+      <c r="M22" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="N22" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="10">
+      <c r="N22" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1421,7 +1412,7 @@
       <c r="D23" s="6">
         <v>5</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="6">
         <v>5</v>
       </c>
       <c r="H23" s="6">
@@ -1431,19 +1422,19 @@
       <c r="K23" s="2">
         <v>5</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="8">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="N23" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P23" s="10">
+      <c r="N23" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P23" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1459,35 +1450,35 @@
         <v>20</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="D24" s="6">
+        <v>5</v>
+      </c>
+      <c r="E24" s="6">
         <v>5</v>
       </c>
       <c r="H24" s="6">
         <v>5</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="7">
         <v>5</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2">
         <v>5</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="8">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="N24" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P24" s="10">
+      <c r="N24" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P24" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1502,20 +1493,20 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="6">
         <v>5</v>
       </c>
       <c r="D25" s="6">
         <v>5</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2">
-        <v>5</v>
-      </c>
-      <c r="I25">
+      <c r="F25" s="7">
+        <v>5</v>
+      </c>
+      <c r="H25" s="6">
+        <v>5</v>
+      </c>
+      <c r="I25" s="7">
         <v>5</v>
       </c>
       <c r="J25" s="2">
@@ -1524,19 +1515,19 @@
       <c r="K25" s="2">
         <v>5</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="8">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="N25" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O25" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P25" s="10">
+      <c r="N25" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O25" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P25" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1565,19 +1556,19 @@
       <c r="K26" s="6">
         <v>5</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="N26" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="10">
+      <c r="N26" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1606,19 +1597,19 @@
       <c r="K27" s="6">
         <v>5</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="N27" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="10">
+      <c r="N27" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1633,7 +1624,7 @@
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="6">
         <v>5</v>
       </c>
       <c r="D28" s="6">
@@ -1643,26 +1634,26 @@
       <c r="H28" s="6">
         <v>5</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="7">
         <v>5</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="6">
         <v>5</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28" s="8">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="N28" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P28" s="10">
+      <c r="N28" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P28" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1683,38 +1674,38 @@
       <c r="D29" s="6">
         <v>5</v>
       </c>
-      <c r="E29" s="2">
-        <v>5</v>
-      </c>
-      <c r="F29">
-        <v>5</v>
-      </c>
-      <c r="G29">
+      <c r="E29" s="6">
+        <v>5</v>
+      </c>
+      <c r="F29" s="7">
+        <v>5</v>
+      </c>
+      <c r="G29" s="7">
         <v>5</v>
       </c>
       <c r="H29" s="6">
         <v>5</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="7">
         <v>5</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2">
         <v>5</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="8">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="N29" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O29" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P29" s="10">
+      <c r="N29" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O29" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P29" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1733,7 +1724,7 @@
       <c r="D30" s="6">
         <v>5</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="6">
         <v>5</v>
       </c>
       <c r="H30" s="6">
@@ -1743,19 +1734,19 @@
       <c r="K30" s="2">
         <v>5</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="N30" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="10">
+      <c r="N30" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1780,19 +1771,19 @@
         <v>10</v>
       </c>
       <c r="K31" s="2"/>
-      <c r="M31" s="10">
+      <c r="M31" s="8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="N31" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O31" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P31" s="10">
+      <c r="N31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1816,35 +1807,35 @@
       <c r="E32" s="6">
         <v>5</v>
       </c>
-      <c r="F32" s="8">
-        <v>5</v>
-      </c>
-      <c r="G32" s="8">
+      <c r="F32" s="11">
+        <v>5</v>
+      </c>
+      <c r="G32" s="11">
         <v>5</v>
       </c>
       <c r="H32" s="6">
         <v>5</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="11">
         <v>5</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2">
         <v>5</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="8">
         <f>SUM(C32:K32)</f>
         <v>40</v>
       </c>
-      <c r="N32" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O32" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P32" s="10">
+      <c r="N32" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O32" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P32" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_19 ноября 2023 г. 15:10:22_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -246,14 +246,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -561,10 +561,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
+      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -575,29 +575,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -691,7 +691,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="2">
+      <c r="K5" s="6">
         <v>5</v>
       </c>
       <c r="M5">
@@ -732,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="2">
+      <c r="K6" s="6">
         <v>5</v>
       </c>
       <c r="M6" s="8">
@@ -773,7 +773,7 @@
         <v>5</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="2">
+      <c r="K7" s="6">
         <v>3</v>
       </c>
       <c r="M7" s="8">
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="2">
+      <c r="K8" s="6">
         <v>4</v>
       </c>
       <c r="M8" s="8">
@@ -896,7 +896,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="2">
+      <c r="K10" s="6">
         <v>5</v>
       </c>
       <c r="M10" s="8">
@@ -1018,7 +1018,7 @@
         <v>5</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="K13" s="2">
+      <c r="K13" s="6">
         <v>5</v>
       </c>
       <c r="M13" s="8">
@@ -1101,7 +1101,7 @@
         <v>5</v>
       </c>
       <c r="J15" s="2"/>
-      <c r="K15" s="2">
+      <c r="K15" s="6">
         <v>5</v>
       </c>
       <c r="M15" s="8">
@@ -1181,7 +1181,7 @@
         <v>5</v>
       </c>
       <c r="J17" s="2"/>
-      <c r="K17" s="2">
+      <c r="K17" s="6">
         <v>4</v>
       </c>
       <c r="M17" s="8">
@@ -1223,7 +1223,7 @@
         <v>5</v>
       </c>
       <c r="J18" s="2"/>
-      <c r="K18" s="2">
+      <c r="K18" s="6">
         <v>5</v>
       </c>
       <c r="M18" s="8">
@@ -1331,7 +1331,7 @@
       <c r="H21" s="6">
         <v>5</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="10">
         <v>5</v>
       </c>
       <c r="J21" s="2"/>
@@ -1419,7 +1419,7 @@
         <v>5</v>
       </c>
       <c r="J23" s="2"/>
-      <c r="K23" s="2">
+      <c r="K23" s="6">
         <v>5</v>
       </c>
       <c r="M23" s="8">
@@ -1463,7 +1463,7 @@
         <v>5</v>
       </c>
       <c r="J24" s="2"/>
-      <c r="K24" s="2">
+      <c r="K24" s="6">
         <v>5</v>
       </c>
       <c r="M24" s="8">
@@ -1509,10 +1509,10 @@
       <c r="I25" s="7">
         <v>5</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="6">
         <v>10</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="6">
         <v>5</v>
       </c>
       <c r="M25" s="8">
@@ -1690,7 +1690,7 @@
         <v>5</v>
       </c>
       <c r="J29" s="2"/>
-      <c r="K29" s="2">
+      <c r="K29" s="6">
         <v>5</v>
       </c>
       <c r="M29" s="8">
@@ -1731,7 +1731,7 @@
         <v>5</v>
       </c>
       <c r="J30" s="2"/>
-      <c r="K30" s="2">
+      <c r="K30" s="6">
         <v>5</v>
       </c>
       <c r="M30" s="8">
@@ -1807,20 +1807,20 @@
       <c r="E32" s="6">
         <v>5</v>
       </c>
-      <c r="F32" s="11">
-        <v>5</v>
-      </c>
-      <c r="G32" s="11">
+      <c r="F32" s="9">
+        <v>5</v>
+      </c>
+      <c r="G32" s="9">
         <v>5</v>
       </c>
       <c r="H32" s="6">
         <v>5</v>
       </c>
-      <c r="I32" s="11">
+      <c r="I32" s="9">
         <v>5</v>
       </c>
       <c r="J32" s="2"/>
-      <c r="K32" s="2">
+      <c r="K32" s="6">
         <v>5</v>
       </c>
       <c r="M32" s="8">

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 21:22:53_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -561,10 +561,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -969,7 +969,9 @@
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
       <c r="D12" s="6">
         <v>5</v>
       </c>
@@ -983,7 +985,7 @@
       <c r="K12" s="2"/>
       <c r="M12" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="N12" s="8">
         <f t="shared" si="2"/>
@@ -995,7 +997,7 @@
       </c>
       <c r="P12" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 21:54:54_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -561,10 +561,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1010,9 @@
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="7">
@@ -1025,7 +1027,7 @@
       </c>
       <c r="M13" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="N13" s="8">
         <f t="shared" si="2"/>
@@ -1037,7 +1039,7 @@
       </c>
       <c r="P13" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13">
         <v>3</v>
@@ -1585,7 +1587,9 @@
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
       <c r="D27" s="6">
         <v>5</v>
       </c>
@@ -1601,7 +1605,7 @@
       </c>
       <c r="M27" s="8">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N27" s="8">
         <f t="shared" si="2"/>
@@ -1609,7 +1613,7 @@
       </c>
       <c r="O27" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" si="2"/>
@@ -1632,7 +1636,9 @@
       <c r="D28" s="6">
         <v>5</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2">
+        <v>5</v>
+      </c>
       <c r="H28" s="6">
         <v>5</v>
       </c>
@@ -1645,11 +1651,11 @@
       </c>
       <c r="M28" s="8">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="N28" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="8">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 22:03:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -574,10 +574,10 @@
   <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1249,7 +1249,9 @@
       <c r="F26">
         <v>5</v>
       </c>
-      <c r="H26" s="12"/>
+      <c r="H26" s="12">
+        <v>5</v>
+      </c>
       <c r="I26" s="6">
         <v>5</v>
       </c>
@@ -1342,7 +1344,9 @@
       <c r="G29" s="7">
         <v>5</v>
       </c>
-      <c r="H29" s="12"/>
+      <c r="H29" s="12">
+        <v>5</v>
+      </c>
       <c r="I29" s="6">
         <v>5</v>
       </c>
@@ -1427,7 +1431,9 @@
       <c r="G32" s="9">
         <v>5</v>
       </c>
-      <c r="H32" s="12"/>
+      <c r="H32" s="12">
+        <v>5</v>
+      </c>
       <c r="I32" s="6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 22:05:00_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -577,7 +577,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
+      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1255,7 +1255,12 @@
       <c r="I26" s="6">
         <v>5</v>
       </c>
-      <c r="K26" s="2"/>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26" s="2">
+        <v>5</v>
+      </c>
       <c r="L26" s="6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_3 декабря 2023 г. 22:07:54_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>2ОИБАС1222: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Инд6</t>
+  </si>
+  <si>
+    <t>Инд7</t>
+  </si>
+  <si>
+    <t>Инд8</t>
   </si>
 </sst>
 </file>
@@ -574,10 +580,10 @@
   <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -633,18 +639,24 @@
         <v>41</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="1"/>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="1">
@@ -662,16 +674,18 @@
       <c r="G4" s="4">
         <v>5</v>
       </c>
-      <c r="I4" s="1">
-        <v>5</v>
-      </c>
-      <c r="J4" s="4">
-        <v>5</v>
-      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
       <c r="K4" s="1">
+        <v>5</v>
+      </c>
+      <c r="L4" s="4">
+        <v>5</v>
+      </c>
+      <c r="M4" s="1">
         <v>10</v>
       </c>
-      <c r="L4" s="1">
+      <c r="N4" s="1">
         <v>5</v>
       </c>
     </row>
@@ -691,15 +705,15 @@
         <v>5</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="6">
-        <v>5</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="6">
-        <v>5</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="6">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -716,15 +730,15 @@
         <v>5</v>
       </c>
       <c r="H6" s="12"/>
-      <c r="I6" s="6">
-        <v>5</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="6">
-        <v>5</v>
-      </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="6">
+        <v>5</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="6">
+        <v>5</v>
+      </c>
       <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -742,15 +756,15 @@
         <v>5</v>
       </c>
       <c r="H7" s="12"/>
-      <c r="I7" s="6">
-        <v>5</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="6">
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="6">
+        <v>5</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="6">
         <v>3</v>
       </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
       <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -766,15 +780,15 @@
       </c>
       <c r="E8" s="2"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="6">
-        <v>5</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="6">
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="6">
+        <v>5</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="6">
         <v>4</v>
       </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
       <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -793,13 +807,13 @@
         <v>5</v>
       </c>
       <c r="H9" s="12"/>
-      <c r="I9" s="6">
-        <v>5</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="6">
+        <v>5</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
       <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -817,18 +831,18 @@
       </c>
       <c r="E10" s="2"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="6">
-        <v>5</v>
-      </c>
-      <c r="J10" s="7">
-        <v>5</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="6">
-        <v>5</v>
-      </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="6">
+        <v>5</v>
+      </c>
+      <c r="L10" s="7">
+        <v>5</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="6">
+        <v>5</v>
+      </c>
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -850,15 +864,15 @@
       <c r="H11" s="11">
         <v>5</v>
       </c>
-      <c r="I11" s="6">
-        <v>5</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="6">
-        <v>5</v>
-      </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="6">
+        <v>5</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="6">
+        <v>5</v>
+      </c>
       <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -878,13 +892,13 @@
         <v>5</v>
       </c>
       <c r="H12" s="12"/>
-      <c r="I12" s="6">
-        <v>5</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="6">
+        <v>5</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
       <c r="P12" s="8"/>
     </row>
     <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -903,15 +917,15 @@
         <v>5</v>
       </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="6">
-        <v>5</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="6">
-        <v>5</v>
-      </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="6">
+        <v>5</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="6">
+        <v>5</v>
+      </c>
       <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -931,13 +945,13 @@
       <c r="H14" s="12">
         <v>5</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="6">
-        <v>5</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="6">
+        <v>5</v>
+      </c>
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -957,16 +971,16 @@
         <v>5</v>
       </c>
       <c r="H15" s="12"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="7">
-        <v>5</v>
-      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="6">
-        <v>5</v>
-      </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="L15" s="7">
+        <v>5</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="6">
+        <v>5</v>
+      </c>
       <c r="P15" s="8"/>
     </row>
     <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -986,13 +1000,13 @@
         <v>5</v>
       </c>
       <c r="H16" s="12"/>
-      <c r="I16" s="6">
-        <v>5</v>
-      </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="6">
+        <v>5</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1008,15 +1022,15 @@
       </c>
       <c r="E17" s="2"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="6">
-        <v>5</v>
-      </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="6">
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="6">
+        <v>5</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="6">
         <v>4</v>
       </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
       <c r="P17" s="8"/>
     </row>
     <row r="18" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1032,18 +1046,18 @@
         <v>5</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="6">
-        <v>5</v>
-      </c>
-      <c r="J18" s="7">
-        <v>5</v>
-      </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="6">
-        <v>5</v>
-      </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="6">
+        <v>5</v>
+      </c>
+      <c r="L18" s="7">
+        <v>5</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="6">
+        <v>5</v>
+      </c>
       <c r="P18" s="8"/>
     </row>
     <row r="19" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1057,11 +1071,11 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="2"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
       <c r="P19" s="8"/>
     </row>
     <row r="20" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1075,11 +1089,11 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
       <c r="P20" s="8"/>
     </row>
     <row r="21" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1099,18 +1113,18 @@
         <v>5</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="6">
-        <v>5</v>
-      </c>
-      <c r="J21" s="10">
-        <v>5</v>
-      </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="6">
-        <v>5</v>
-      </c>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="6">
+        <v>5</v>
+      </c>
+      <c r="L21" s="10">
+        <v>5</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="6">
+        <v>5</v>
+      </c>
       <c r="P21" s="8"/>
     </row>
     <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1130,13 +1144,13 @@
         <v>5</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="6">
-        <v>5</v>
-      </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="6">
+        <v>5</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
       <c r="P22" s="8"/>
     </row>
     <row r="23" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1158,15 +1172,15 @@
       <c r="H23" s="12">
         <v>5</v>
       </c>
-      <c r="I23" s="6">
-        <v>5</v>
-      </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="6">
-        <v>5</v>
-      </c>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="6">
+        <v>5</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="6">
+        <v>5</v>
+      </c>
       <c r="P23" s="8"/>
     </row>
     <row r="24" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1184,18 +1198,18 @@
         <v>5</v>
       </c>
       <c r="H24" s="12"/>
-      <c r="I24" s="6">
-        <v>5</v>
-      </c>
-      <c r="J24" s="7">
-        <v>5</v>
-      </c>
-      <c r="K24" s="2"/>
-      <c r="L24" s="6">
-        <v>5</v>
-      </c>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="6">
+        <v>5</v>
+      </c>
+      <c r="L24" s="7">
+        <v>5</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="6">
+        <v>5</v>
+      </c>
       <c r="P24" s="8"/>
     </row>
     <row r="25" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1216,20 +1230,20 @@
         <v>5</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="6">
-        <v>5</v>
-      </c>
-      <c r="J25" s="7">
-        <v>5</v>
-      </c>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
       <c r="K25" s="6">
+        <v>5</v>
+      </c>
+      <c r="L25" s="7">
+        <v>5</v>
+      </c>
+      <c r="M25" s="6">
         <v>10</v>
       </c>
-      <c r="L25" s="6">
-        <v>5</v>
-      </c>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
+      <c r="N25" s="6">
+        <v>5</v>
+      </c>
       <c r="P25" s="8"/>
     </row>
     <row r="26" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1252,20 +1266,20 @@
       <c r="H26" s="12">
         <v>5</v>
       </c>
-      <c r="I26" s="6">
-        <v>5</v>
-      </c>
-      <c r="J26">
-        <v>5</v>
-      </c>
-      <c r="K26" s="2">
-        <v>5</v>
-      </c>
-      <c r="L26" s="6">
-        <v>5</v>
-      </c>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="6">
+        <v>5</v>
+      </c>
+      <c r="L26">
+        <v>5</v>
+      </c>
+      <c r="M26" s="2">
+        <v>5</v>
+      </c>
+      <c r="N26" s="6">
+        <v>5</v>
+      </c>
       <c r="P26" s="8"/>
     </row>
     <row r="27" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1285,15 +1299,15 @@
         <v>5</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="6">
-        <v>5</v>
-      </c>
-      <c r="K27" s="2"/>
-      <c r="L27" s="6">
-        <v>5</v>
-      </c>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="6">
+        <v>5</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="6">
+        <v>5</v>
+      </c>
       <c r="P27" s="8"/>
     </row>
     <row r="28" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1313,18 +1327,18 @@
         <v>5</v>
       </c>
       <c r="H28" s="12"/>
-      <c r="I28" s="6">
-        <v>5</v>
-      </c>
-      <c r="J28" s="7">
-        <v>5</v>
-      </c>
-      <c r="K28" s="2"/>
-      <c r="L28" s="6">
-        <v>5</v>
-      </c>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="6">
+        <v>5</v>
+      </c>
+      <c r="L28" s="7">
+        <v>5</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="6">
+        <v>5</v>
+      </c>
       <c r="P28" s="8"/>
     </row>
     <row r="29" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1352,18 +1366,20 @@
       <c r="H29" s="12">
         <v>5</v>
       </c>
-      <c r="I29" s="6">
-        <v>5</v>
-      </c>
-      <c r="J29" s="7">
-        <v>5</v>
-      </c>
-      <c r="K29" s="2"/>
-      <c r="L29" s="6">
-        <v>5</v>
-      </c>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
+      <c r="I29" s="12">
+        <v>5</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="K29" s="6">
+        <v>5</v>
+      </c>
+      <c r="L29" s="7">
+        <v>5</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="6">
+        <v>5</v>
+      </c>
       <c r="P29" s="8"/>
     </row>
     <row r="30" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1381,15 +1397,15 @@
         <v>5</v>
       </c>
       <c r="H30" s="12"/>
-      <c r="I30" s="6">
-        <v>5</v>
-      </c>
-      <c r="K30" s="2"/>
-      <c r="L30" s="6">
-        <v>5</v>
-      </c>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="6">
+        <v>5</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="6">
+        <v>5</v>
+      </c>
       <c r="P30" s="8"/>
     </row>
     <row r="31" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1403,15 +1419,15 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="6">
-        <v>5</v>
-      </c>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
       <c r="K31" s="6">
+        <v>5</v>
+      </c>
+      <c r="M31" s="6">
         <v>10</v>
       </c>
-      <c r="L31" s="2"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
+      <c r="N31" s="2"/>
       <c r="P31" s="8"/>
     </row>
     <row r="32" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1439,39 +1455,47 @@
       <c r="H32" s="12">
         <v>5</v>
       </c>
-      <c r="I32" s="6">
-        <v>5</v>
-      </c>
-      <c r="J32" s="9">
-        <v>5</v>
-      </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="6">
-        <v>5</v>
-      </c>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
+      <c r="I32" s="12">
+        <v>5</v>
+      </c>
+      <c r="J32" s="12">
+        <v>5</v>
+      </c>
+      <c r="K32" s="6">
+        <v>5</v>
+      </c>
+      <c r="L32" s="9">
+        <v>5</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="6">
+        <v>5</v>
+      </c>
       <c r="P32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="H33" s="12"/>
-      <c r="I33" s="3"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="2:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" spans="2:14" ht="13" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H34" s="12"/>
-      <c r="I34" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" ht="13" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>38</v>
       </c>
@@ -1479,8 +1503,10 @@
         <v>5</v>
       </c>
       <c r="H35" s="12"/>
-    </row>
-    <row r="36" spans="2:12" ht="13" x14ac:dyDescent="0.25">
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" spans="2:14" ht="13" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>39</v>
       </c>
@@ -1488,41 +1514,55 @@
         <v>5</v>
       </c>
       <c r="H36" s="12"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H37" s="12"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H38" s="12"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H39" s="12"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H40" s="12"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H41" s="12"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H42" s="12"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H43" s="12"/>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H44" s="12"/>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H45" s="12"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H46" s="12"/>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H47" s="12"/>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H48" s="12"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.25">
@@ -1557,7 +1597,7 @@
   <mergeCells count="1">
     <mergeCell ref="C1:W1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N5:P32">
+  <conditionalFormatting sqref="P5:P32">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_18 декабря 2023 г. 0:07:21_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -181,7 +181,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,8 +200,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -235,11 +241,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -271,6 +286,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -583,7 +601,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -594,29 +612,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
     </row>
     <row r="2" spans="1:23" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1043,6 +1061,12 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="6">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
         <v>5</v>
       </c>
       <c r="H18" s="12"/>
@@ -1112,7 +1136,12 @@
       <c r="E21" s="6">
         <v>5</v>
       </c>
-      <c r="H21" s="12"/>
+      <c r="G21" s="13">
+        <v>5</v>
+      </c>
+      <c r="H21" s="12">
+        <v>5</v>
+      </c>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="6">
@@ -1261,6 +1290,9 @@
         <v>5</v>
       </c>
       <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
         <v>5</v>
       </c>
       <c r="H26" s="12">

</xml_diff>

<commit_message>
AutoCommit_18 декабря 2023 г. 9:48:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -598,10 +598,10 @@
   <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -882,7 +882,9 @@
       <c r="H11" s="11">
         <v>5</v>
       </c>
-      <c r="I11" s="12"/>
+      <c r="I11" s="12">
+        <v>5</v>
+      </c>
       <c r="J11" s="12"/>
       <c r="K11" s="6">
         <v>5</v>
@@ -1142,7 +1144,9 @@
       <c r="H21" s="12">
         <v>5</v>
       </c>
-      <c r="I21" s="12"/>
+      <c r="I21" s="12">
+        <v>5</v>
+      </c>
       <c r="J21" s="12"/>
       <c r="K21" s="6">
         <v>5</v>
@@ -1298,7 +1302,9 @@
       <c r="H26" s="12">
         <v>5</v>
       </c>
-      <c r="I26" s="12"/>
+      <c r="I26" s="12">
+        <v>5</v>
+      </c>
       <c r="J26" s="12"/>
       <c r="K26" s="6">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_18 декабря 2023 г. 9:56:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -598,10 +598,10 @@
   <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -885,7 +885,9 @@
       <c r="I11" s="12">
         <v>5</v>
       </c>
-      <c r="J11" s="12"/>
+      <c r="J11" s="12">
+        <v>5</v>
+      </c>
       <c r="K11" s="6">
         <v>5</v>
       </c>
@@ -1147,7 +1149,9 @@
       <c r="I21" s="12">
         <v>5</v>
       </c>
-      <c r="J21" s="12"/>
+      <c r="J21" s="12">
+        <v>5</v>
+      </c>
       <c r="K21" s="6">
         <v>5</v>
       </c>
@@ -1305,7 +1309,9 @@
       <c r="I26" s="12">
         <v>5</v>
       </c>
-      <c r="J26" s="12"/>
+      <c r="J26" s="12">
+        <v>5</v>
+      </c>
       <c r="K26" s="6">
         <v>5</v>
       </c>
@@ -1407,7 +1413,9 @@
       <c r="I29" s="12">
         <v>5</v>
       </c>
-      <c r="J29" s="12"/>
+      <c r="J29" s="12">
+        <v>5</v>
+      </c>
       <c r="K29" s="6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_28 декабря 2023 г. 12:11:08_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>2ОИБАС1222: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Инд8</t>
+  </si>
+  <si>
+    <t>Сумма</t>
   </si>
 </sst>
 </file>
@@ -240,7 +243,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -256,6 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -560,13 +563,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I40" sqref="I40:K40"/>
+      <selection pane="bottomRight" activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -577,12 +580,12 @@
     <col min="4" max="9" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="10" t="s">
+    <row r="1" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
@@ -621,26 +624,29 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="H3" s="3"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>IF(B4=C4,A3+1,"-------------------")</f>
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -654,9 +660,9 @@
       <c r="G4" s="5">
         <v>5</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
       <c r="L4" s="4">
         <v>5</v>
       </c>
@@ -664,13 +670,20 @@
       <c r="O4" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q4">
+        <f>SUM(D4:O4)</f>
+        <v>20</v>
+      </c>
+      <c r="R4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A31" si="0">IF(B5=C5,A4+1,"-------------------")</f>
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -683,9 +696,9 @@
       <c r="F5" s="4">
         <v>5</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
       <c r="L5" s="4">
         <v>5</v>
       </c>
@@ -693,14 +706,20 @@
       <c r="O5" s="4">
         <v>5</v>
       </c>
-      <c r="Q5" s="6"/>
-    </row>
-    <row r="6" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q5" s="9">
+        <f t="shared" ref="Q5:Q40" si="1">SUM(D5:O5)</f>
+        <v>20</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -713,9 +732,9 @@
       <c r="F6" s="4">
         <v>5</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
       <c r="L6" s="4">
         <v>5</v>
       </c>
@@ -723,14 +742,20 @@
       <c r="O6" s="4">
         <v>3</v>
       </c>
-      <c r="Q6" s="6"/>
-    </row>
-    <row r="7" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q6" s="9">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -741,9 +766,9 @@
         <v>5</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
       <c r="L7" s="4">
         <v>5</v>
       </c>
@@ -751,14 +776,20 @@
       <c r="O7" s="4">
         <v>4</v>
       </c>
-      <c r="Q7" s="6"/>
-    </row>
-    <row r="8" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q7" s="9">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -772,22 +803,28 @@
       <c r="G8" s="5">
         <v>5</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
       <c r="L8" s="4">
         <v>5</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q8" s="9">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="R8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -800,9 +837,9 @@
         <v>5</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
       <c r="L9" s="4">
         <v>5</v>
       </c>
@@ -813,14 +850,20 @@
       <c r="O9" s="4">
         <v>5</v>
       </c>
-      <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q9" s="9">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -851,14 +894,20 @@
       <c r="O10" s="4">
         <v>5</v>
       </c>
-      <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q10" s="9">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="R10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -873,22 +922,28 @@
       <c r="F11" s="4">
         <v>5</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
       <c r="L11" s="4">
         <v>5</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q11" s="9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -902,9 +957,9 @@
       <c r="G12" s="5">
         <v>5</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="4">
         <v>5</v>
       </c>
@@ -912,14 +967,20 @@
       <c r="O12" s="4">
         <v>5</v>
       </c>
-      <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q12" s="9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -935,21 +996,27 @@
       <c r="I13" s="4">
         <v>5</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
       <c r="L13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="4">
         <v>5</v>
       </c>
-      <c r="Q13" s="6"/>
-    </row>
-    <row r="14" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13" s="9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="R13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -964,9 +1031,9 @@
       <c r="F14" s="4">
         <v>5</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
       <c r="L14" s="2"/>
       <c r="M14" s="5">
         <v>5</v>
@@ -975,14 +1042,20 @@
       <c r="O14" s="4">
         <v>5</v>
       </c>
-      <c r="Q14" s="6"/>
-    </row>
-    <row r="15" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q14" s="9">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="R14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -997,22 +1070,28 @@
       <c r="F15" s="4">
         <v>5</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
       <c r="L15" s="4">
         <v>5</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="Q15" s="6"/>
-    </row>
-    <row r="16" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q15" s="9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1023,9 +1102,9 @@
         <v>5</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
       <c r="L16" s="4">
         <v>5</v>
       </c>
@@ -1033,14 +1112,20 @@
       <c r="O16" s="4">
         <v>4</v>
       </c>
-      <c r="Q16" s="6"/>
-    </row>
-    <row r="17" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="9">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="R16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1057,9 +1142,9 @@
       <c r="H17" s="4">
         <v>5</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
       <c r="L17" s="4">
         <v>5</v>
       </c>
@@ -1070,50 +1155,70 @@
       <c r="O17" s="4">
         <v>5</v>
       </c>
-      <c r="Q17" s="6"/>
-    </row>
-    <row r="18" spans="1:17" s="12" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
+      <c r="Q17" s="9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="R17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-    </row>
-    <row r="19" spans="1:17" s="12" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="Q18" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-    </row>
-    <row r="20" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="Q19" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1143,21 +1248,27 @@
       <c r="L20" s="4">
         <v>5</v>
       </c>
-      <c r="M20" s="8">
+      <c r="M20" s="7">
         <v>5</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="4">
         <v>5</v>
       </c>
-      <c r="Q20" s="6"/>
-    </row>
-    <row r="21" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q20" s="9">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1172,22 +1283,28 @@
       <c r="F21" s="4">
         <v>5</v>
       </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
       <c r="L21" s="4">
         <v>5</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="Q21" s="6"/>
-    </row>
-    <row r="22" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q21" s="9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="R21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1205,8 +1322,8 @@
       <c r="I22" s="4">
         <v>5</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
       <c r="L22" s="4">
         <v>5</v>
       </c>
@@ -1214,14 +1331,20 @@
       <c r="O22" s="4">
         <v>5</v>
       </c>
-      <c r="Q22" s="6"/>
-    </row>
-    <row r="23" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q22" s="9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="R22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1234,9 +1357,9 @@
       <c r="F23" s="4">
         <v>5</v>
       </c>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
       <c r="L23" s="4">
         <v>5</v>
       </c>
@@ -1247,14 +1370,20 @@
       <c r="O23" s="4">
         <v>5</v>
       </c>
-      <c r="Q23" s="6"/>
-    </row>
-    <row r="24" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q23" s="9">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="R23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1270,9 +1399,9 @@
       <c r="G24" s="5">
         <v>5</v>
       </c>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
       <c r="L24" s="4">
         <v>5</v>
       </c>
@@ -1280,19 +1409,25 @@
         <v>5</v>
       </c>
       <c r="N24" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O24" s="4">
         <v>5</v>
       </c>
-      <c r="Q24" s="6"/>
-    </row>
-    <row r="25" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q24" s="9">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="R24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1323,23 +1458,29 @@
       <c r="L25" s="4">
         <v>5</v>
       </c>
-      <c r="M25">
-        <v>5</v>
-      </c>
-      <c r="N25" s="2">
+      <c r="M25" s="4">
+        <v>5</v>
+      </c>
+      <c r="N25" s="4">
         <v>5</v>
       </c>
       <c r="O25" s="4">
         <v>5</v>
       </c>
-      <c r="Q25" s="6"/>
-    </row>
-    <row r="26" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q25" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R25" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1354,9 +1495,9 @@
       <c r="F26" s="4">
         <v>5</v>
       </c>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
       <c r="L26" s="4">
         <v>5</v>
       </c>
@@ -1364,14 +1505,20 @@
       <c r="O26" s="4">
         <v>5</v>
       </c>
-      <c r="Q26" s="6"/>
-    </row>
-    <row r="27" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q26" s="9">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="R26" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1386,9 +1533,9 @@
       <c r="F27" s="4">
         <v>5</v>
       </c>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
       <c r="L27" s="4">
         <v>5</v>
       </c>
@@ -1399,14 +1546,20 @@
       <c r="O27" s="4">
         <v>5</v>
       </c>
-      <c r="Q27" s="6"/>
-    </row>
-    <row r="28" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q27" s="9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="R27" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1446,14 +1599,20 @@
       <c r="O28" s="4">
         <v>5</v>
       </c>
-      <c r="Q28" s="6"/>
-    </row>
-    <row r="29" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q28" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1466,9 +1625,9 @@
       <c r="F29" s="4">
         <v>5</v>
       </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
       <c r="L29" s="4">
         <v>5</v>
       </c>
@@ -1476,14 +1635,20 @@
       <c r="O29" s="4">
         <v>5</v>
       </c>
-      <c r="Q29" s="6"/>
-    </row>
-    <row r="30" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q29" s="9">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="R29" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1492,24 +1657,30 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
       <c r="L30" s="4">
         <v>5</v>
       </c>
       <c r="N30" s="4">
+        <v>5</v>
+      </c>
+      <c r="O30" s="2"/>
+      <c r="Q30" s="9">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="O30" s="2"/>
-      <c r="Q30" s="6"/>
-    </row>
-    <row r="31" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R30" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1524,10 +1695,10 @@
       <c r="F31" s="4">
         <v>5</v>
       </c>
-      <c r="G31" s="7">
-        <v>5</v>
-      </c>
-      <c r="H31" s="7">
+      <c r="G31" s="6">
+        <v>5</v>
+      </c>
+      <c r="H31" s="6">
         <v>5</v>
       </c>
       <c r="I31" s="4">
@@ -1542,16 +1713,22 @@
       <c r="L31" s="4">
         <v>5</v>
       </c>
-      <c r="M31" s="7">
+      <c r="M31" s="6">
         <v>5</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="4">
         <v>5</v>
       </c>
-      <c r="Q31" s="6"/>
-    </row>
-    <row r="32" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q31" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>28</v>
       </c>
@@ -1564,10 +1741,10 @@
       <c r="F32" s="4">
         <v>5</v>
       </c>
-      <c r="G32" s="7">
-        <v>5</v>
-      </c>
-      <c r="H32" s="7">
+      <c r="G32" s="6">
+        <v>5</v>
+      </c>
+      <c r="H32" s="6">
         <v>5</v>
       </c>
       <c r="I32" s="4">
@@ -1582,15 +1759,22 @@
       <c r="L32" s="4">
         <v>5</v>
       </c>
-      <c r="M32" s="7">
+      <c r="M32" s="6">
         <v>5</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="3:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q32" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
         <v>28</v>
       </c>
@@ -1603,10 +1787,10 @@
       <c r="F33" s="4">
         <v>5</v>
       </c>
-      <c r="G33" s="7">
-        <v>5</v>
-      </c>
-      <c r="H33" s="7">
+      <c r="G33" s="6">
+        <v>5</v>
+      </c>
+      <c r="H33" s="6">
         <v>5</v>
       </c>
       <c r="I33" s="4">
@@ -1621,15 +1805,22 @@
       <c r="L33" s="4">
         <v>5</v>
       </c>
-      <c r="M33" s="7">
+      <c r="M33" s="6">
         <v>5</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="3:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q33" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>28</v>
       </c>
@@ -1642,10 +1833,10 @@
       <c r="F34" s="4">
         <v>5</v>
       </c>
-      <c r="G34" s="7">
-        <v>5</v>
-      </c>
-      <c r="H34" s="7">
+      <c r="G34" s="6">
+        <v>5</v>
+      </c>
+      <c r="H34" s="6">
         <v>5</v>
       </c>
       <c r="I34" s="4">
@@ -1660,15 +1851,22 @@
       <c r="L34" s="4">
         <v>5</v>
       </c>
-      <c r="M34" s="7">
+      <c r="M34" s="6">
         <v>5</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="3:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q34" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
         <v>28</v>
       </c>
@@ -1681,10 +1879,10 @@
       <c r="F35" s="4">
         <v>5</v>
       </c>
-      <c r="G35" s="7">
-        <v>5</v>
-      </c>
-      <c r="H35" s="7">
+      <c r="G35" s="6">
+        <v>5</v>
+      </c>
+      <c r="H35" s="6">
         <v>5</v>
       </c>
       <c r="I35" s="4">
@@ -1699,15 +1897,22 @@
       <c r="L35" s="4">
         <v>5</v>
       </c>
-      <c r="M35" s="7">
+      <c r="M35" s="6">
         <v>5</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="3:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q35" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
         <v>28</v>
       </c>
@@ -1720,10 +1925,10 @@
       <c r="F36" s="4">
         <v>5</v>
       </c>
-      <c r="G36" s="7">
-        <v>5</v>
-      </c>
-      <c r="H36" s="7">
+      <c r="G36" s="6">
+        <v>5</v>
+      </c>
+      <c r="H36" s="6">
         <v>5</v>
       </c>
       <c r="I36" s="4">
@@ -1738,15 +1943,22 @@
       <c r="L36" s="4">
         <v>5</v>
       </c>
-      <c r="M36" s="7">
+      <c r="M36" s="6">
         <v>5</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="3:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q36" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
         <v>28</v>
       </c>
@@ -1759,10 +1971,10 @@
       <c r="F37" s="4">
         <v>5</v>
       </c>
-      <c r="G37" s="7">
-        <v>5</v>
-      </c>
-      <c r="H37" s="7">
+      <c r="G37" s="6">
+        <v>5</v>
+      </c>
+      <c r="H37" s="6">
         <v>5</v>
       </c>
       <c r="I37" s="4">
@@ -1777,15 +1989,22 @@
       <c r="L37" s="4">
         <v>5</v>
       </c>
-      <c r="M37" s="7">
+      <c r="M37" s="6">
         <v>5</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="3:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q37" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
         <v>28</v>
       </c>
@@ -1798,10 +2017,10 @@
       <c r="F38" s="4">
         <v>5</v>
       </c>
-      <c r="G38" s="7">
-        <v>5</v>
-      </c>
-      <c r="H38" s="7">
+      <c r="G38" s="6">
+        <v>5</v>
+      </c>
+      <c r="H38" s="6">
         <v>5</v>
       </c>
       <c r="I38" s="4">
@@ -1816,15 +2035,22 @@
       <c r="L38" s="4">
         <v>5</v>
       </c>
-      <c r="M38" s="7">
+      <c r="M38" s="6">
         <v>5</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="3:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q38" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
         <v>28</v>
       </c>
@@ -1837,10 +2063,10 @@
       <c r="F39" s="4">
         <v>5</v>
       </c>
-      <c r="G39" s="7">
-        <v>5</v>
-      </c>
-      <c r="H39" s="7">
+      <c r="G39" s="6">
+        <v>5</v>
+      </c>
+      <c r="H39" s="6">
         <v>5</v>
       </c>
       <c r="I39" s="4">
@@ -1855,15 +2081,22 @@
       <c r="L39" s="4">
         <v>5</v>
       </c>
-      <c r="M39" s="7">
+      <c r="M39" s="6">
         <v>5</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="3:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q39" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
         <v>28</v>
       </c>
@@ -1876,10 +2109,10 @@
       <c r="F40" s="4">
         <v>5</v>
       </c>
-      <c r="G40" s="7">
-        <v>5</v>
-      </c>
-      <c r="H40" s="7">
+      <c r="G40" s="6">
+        <v>5</v>
+      </c>
+      <c r="H40" s="6">
         <v>5</v>
       </c>
       <c r="I40" s="4">
@@ -1894,67 +2127,74 @@
       <c r="L40" s="4">
         <v>5</v>
       </c>
-      <c r="M40" s="7">
+      <c r="M40" s="6">
         <v>5</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="3:15" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H46" s="9"/>
-    </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H47" s="9"/>
-    </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="H48" s="9"/>
+      <c r="Q40" s="9">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="R40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="3:18" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+    </row>
+    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="H48" s="8"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H49" s="9"/>
+      <c r="H49" s="8"/>
     </row>
     <row r="50" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H50" s="9"/>
+      <c r="H50" s="8"/>
     </row>
     <row r="51" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H51" s="9"/>
+      <c r="H51" s="8"/>
     </row>
     <row r="52" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H52" s="9"/>
+      <c r="H52" s="8"/>
     </row>
     <row r="53" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H53" s="9"/>
+      <c r="H53" s="8"/>
     </row>
     <row r="54" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H54" s="9"/>
+      <c r="H54" s="8"/>
     </row>
     <row r="55" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H55" s="9"/>
+      <c r="H55" s="8"/>
     </row>
     <row r="56" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H56" s="9"/>
+      <c r="H56" s="8"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="Q4:Q31">
+  <conditionalFormatting sqref="Q4:Q40 R25:R27 R29:R30">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_30 декабря 2023 г. 23:55:34_SibNout2021
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\2ОИБАС1222_ОпСис_\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Sibirev I. V." sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -228,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -259,6 +254,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -566,26 +562,26 @@
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M40" sqref="M40"/>
+      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" customWidth="1"/>
-    <col min="4" max="9" width="5.1796875" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="9" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="29.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
@@ -624,7 +620,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -641,7 +637,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>IF(B4=C4,A3+1,"-------------------")</f>
         <v>1</v>
@@ -678,7 +674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A31" si="0">IF(B5=C5,A4+1,"-------------------")</f>
         <v>2</v>
@@ -714,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -750,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -784,7 +780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -819,7 +815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -858,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -902,7 +898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -938,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -975,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1011,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1050,7 +1046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1086,7 +1082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1102,10 +1098,22 @@
         <v>5</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="I16" s="8">
+        <v>5</v>
+      </c>
+      <c r="J16" s="8">
+        <v>5</v>
+      </c>
+      <c r="K16" s="8">
+        <v>5</v>
+      </c>
       <c r="L16" s="4">
+        <v>5</v>
+      </c>
+      <c r="M16" s="14">
         <v>5</v>
       </c>
       <c r="N16" s="2"/>
@@ -1114,13 +1122,13 @@
       </c>
       <c r="Q16" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="R16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1163,7 +1171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" s="11" customFormat="1" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1188,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" s="11" customFormat="1" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1213,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1263,7 +1271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1299,7 +1307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1339,7 +1347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1378,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1422,7 +1430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1475,7 +1483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1513,7 +1521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1554,7 +1562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1607,7 +1615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1643,7 +1651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1657,7 +1665,12 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="I30" s="8"/>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="I30" s="8">
+        <v>5</v>
+      </c>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="4">
@@ -1669,13 +1682,13 @@
       <c r="O30" s="2"/>
       <c r="Q30" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="R30" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1728,7 +1741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
         <v>28</v>
       </c>
@@ -1774,7 +1787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>28</v>
       </c>
@@ -1820,7 +1833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>28</v>
       </c>
@@ -1866,7 +1879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>28</v>
       </c>
@@ -1912,7 +1925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>28</v>
       </c>
@@ -1958,7 +1971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>28</v>
       </c>
@@ -2004,7 +2017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>28</v>
       </c>
@@ -2050,7 +2063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>28</v>
       </c>
@@ -2096,7 +2109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>28</v>
       </c>
@@ -2142,54 +2155,54 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="3:18" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:18" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:18" x14ac:dyDescent="0.2">
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:18" x14ac:dyDescent="0.2">
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:18" x14ac:dyDescent="0.2">
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:18" x14ac:dyDescent="0.2">
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:18" x14ac:dyDescent="0.2">
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:18" x14ac:dyDescent="0.2">
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:18" x14ac:dyDescent="0.2">
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H56" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AutoCommit_30 декабря 2023 г. 23:59:25_SibNout2021
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -559,13 +559,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomRight" activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -576,12 +576,12 @@
     <col min="4" max="9" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="29.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="29.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
@@ -620,7 +620,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -637,7 +637,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>IF(B4=C4,A3+1,"-------------------")</f>
         <v>1</v>
@@ -674,7 +674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A31" si="0">IF(B5=C5,A4+1,"-------------------")</f>
         <v>2</v>
@@ -710,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -746,7 +746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -780,7 +780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -815,7 +815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -854,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -898,7 +898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -934,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -971,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1007,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1046,7 +1046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1082,7 +1082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1126,6 +1126,9 @@
       </c>
       <c r="R16">
         <v>3</v>
+      </c>
+      <c r="S16">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_7 января 2024 г. 15:31:37_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\2ОИБАС1222_ОпСис_\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Sibirev I. V." sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -223,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -254,7 +259,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -559,29 +563,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S56"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S22" sqref="S22"/>
+      <selection pane="bottomRight" activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="9" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+    <col min="4" max="9" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="29.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
@@ -620,7 +624,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -637,7 +641,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>IF(B4=C4,A3+1,"-------------------")</f>
         <v>1</v>
@@ -674,7 +678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A31" si="0">IF(B5=C5,A4+1,"-------------------")</f>
         <v>2</v>
@@ -710,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -746,7 +750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -780,7 +784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -815,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -854,7 +858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -898,7 +902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -934,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -971,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1007,7 +1011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1046,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1082,7 +1086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1098,22 +1102,10 @@
         <v>5</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="G16">
-        <v>5</v>
-      </c>
-      <c r="I16" s="8">
-        <v>5</v>
-      </c>
-      <c r="J16" s="8">
-        <v>5</v>
-      </c>
-      <c r="K16" s="8">
-        <v>5</v>
-      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
       <c r="L16" s="4">
-        <v>5</v>
-      </c>
-      <c r="M16" s="14">
         <v>5</v>
       </c>
       <c r="N16" s="2"/>
@@ -1122,16 +1114,13 @@
       </c>
       <c r="Q16" s="9">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="R16">
         <v>3</v>
       </c>
-      <c r="S16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1174,7 +1163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="11" customFormat="1" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1199,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="11" customFormat="1" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1224,7 +1213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1274,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1310,7 +1299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1350,7 +1339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1389,7 +1378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1433,7 +1422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1486,7 +1475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1524,7 +1513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1565,7 +1554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1618,7 +1607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1654,7 +1643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1668,12 +1657,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30">
-        <v>5</v>
-      </c>
-      <c r="I30" s="8">
-        <v>5</v>
-      </c>
+      <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="4">
@@ -1685,13 +1669,13 @@
       <c r="O30" s="2"/>
       <c r="Q30" s="9">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="R30" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1744,7 +1728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>28</v>
       </c>
@@ -1790,7 +1774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
         <v>28</v>
       </c>
@@ -1836,7 +1820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>28</v>
       </c>
@@ -1882,7 +1866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
         <v>28</v>
       </c>
@@ -1928,7 +1912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
         <v>28</v>
       </c>
@@ -1974,7 +1958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
         <v>28</v>
       </c>
@@ -2020,7 +2004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
         <v>28</v>
       </c>
@@ -2066,7 +2050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
         <v>28</v>
       </c>
@@ -2112,7 +2096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="3:18" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
         <v>28</v>
       </c>
@@ -2158,54 +2142,54 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="3:18" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:18" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H56" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AutoCommit_7 января 2024 г. 16:24:48_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -566,10 +566,10 @@
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M40" sqref="M40"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1102,9 +1102,15 @@
         <v>5</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="I16" s="8">
+        <v>5</v>
+      </c>
+      <c r="J16" s="8">
+        <v>5</v>
+      </c>
+      <c r="K16" s="8">
+        <v>5</v>
+      </c>
       <c r="L16" s="4">
         <v>5</v>
       </c>
@@ -1114,7 +1120,7 @@
       </c>
       <c r="Q16" s="9">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="R16">
         <v>3</v>
@@ -1657,7 +1663,12 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="I30" s="8"/>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="I30" s="8">
+        <v>5</v>
+      </c>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="4">
@@ -1669,7 +1680,7 @@
       <c r="O30" s="2"/>
       <c r="Q30" s="9">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="R30" s="13">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_9 января 2024 г. 10:52:29_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222_ОпСис_/2ОИБАС1222_ОпСис_.xlsx
@@ -569,7 +569,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1123,7 @@
         <v>29</v>
       </c>
       <c r="R16">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>